<commit_message>
add pcb gbr files
</commit_message>
<xml_diff>
--- a/hardware/pcb/BOM.xlsx
+++ b/hardware/pcb/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/Studium/02 Vorlesungen/Semester 06/BA/Umsetzung/hardware/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4E0CE45F-1BE7-CD44-ABC9-AA81278E894B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139F8631-5A28-444E-AB90-BC25AD5F829C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="speaker" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,9 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="vcc_distributor" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/lukas/Documents/Studium/02 Vorlesungen/Semester 06/BA/Umsetzung/hardware/pcb/vcc_distributor/vcc_distributor.csv" decimal="," thousands="." tab="0" semicolon="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="vcc_distributor" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr sourceFile="/Users/lukas/Documents/Studium/02 Vorlesungen/Semester 06/BA/Umsetzung/hardware/pcb/vcc_distributor/vcc_distributor.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t>Id</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Stützkondensator 5V</t>
   </si>
   <si>
-    <t>2 x Stützkondensator 5V, 1 x Stützkondensator 24V, 2x Hochpassfilter 24V</t>
-  </si>
-  <si>
     <t>R9,R8</t>
   </si>
   <si>
@@ -281,13 +278,25 @@
   </si>
   <si>
     <t>I2C Pull-Up</t>
+  </si>
+  <si>
+    <t>C12,C13</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t>Stützkondensator 24 V</t>
+  </si>
+  <si>
+    <t>2 x Stützkondensator 5V, 1 x Stützkondensator 24V, 2x Hochpassfilter 24V (niedrige ESR)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,6 +427,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -764,8 +780,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -825,7 +843,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vcc_distributor" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="vcc_distributor" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1124,11 +1142,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1167,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>69</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1187,7 +1205,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1201,10 +1219,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1213,7 +1231,7 @@
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1221,10 +1239,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1241,7 +1259,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1255,10 +1273,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
         <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>73</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1267,7 +1285,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1278,7 +1296,7 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1295,7 +1313,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1309,7 +1327,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1332,7 +1350,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1361,21 +1379,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1383,70 +1404,67 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
         <v>43</v>
       </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -1455,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
         <v>43</v>
@@ -1463,61 +1481,81 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>38</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1527,10 +1565,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1614,7 +1652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
rework backplate, test circuit
</commit_message>
<xml_diff>
--- a/hardware/pcb/BOM.xlsx
+++ b/hardware/pcb/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/Studium/02 Vorlesungen/Semester 06/BA/Umsetzung/hardware/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443FCA05-01D3-9644-83F6-F594D6A5EAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1EC440-3399-6244-872E-0C6F4C100C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="125">
   <si>
     <t>Id</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>C2,C14,C5, C3</t>
+  </si>
+  <si>
+    <t>x 16</t>
+  </si>
+  <si>
+    <t>x 10</t>
   </si>
 </sst>
 </file>
@@ -1924,7 +1930,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2004,6 +2010,9 @@
       <c r="F3" s="7" t="s">
         <v>88</v>
       </c>
+      <c r="G3" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2079,7 +2088,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>118</v>
@@ -2350,7 +2359,7 @@
         <v>24</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>119</v>
@@ -2400,9 +2409,7 @@
       <c r="F19" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>82</v>
-      </c>
+      <c r="G19" s="7"/>
       <c r="H19" s="8" t="s">
         <v>118</v>
       </c>
@@ -2600,9 +2607,7 @@
       <c r="F27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>82</v>
-      </c>
+      <c r="G27" s="7"/>
       <c r="H27" s="8" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
add software test/analyze methods
</commit_message>
<xml_diff>
--- a/hardware/pcb/BOM.xlsx
+++ b/hardware/pcb/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/Studium/02 Vorlesungen/Semester 06/BA/Umsetzung/hardware/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1EC440-3399-6244-872E-0C6F4C100C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CC7BF3-99C0-B540-BC64-5716521E0CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="speaker" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="126">
   <si>
     <t>Id</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>x 10</t>
+  </si>
+  <si>
+    <t>On Supply</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1927,10 +1930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49091B3E-91A0-044A-8E38-686DA06B527B}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1940,7 +1943,7 @@
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1965,8 +1968,11 @@
       <c r="H1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1989,8 +1995,11 @@
       <c r="H2" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2014,8 +2023,11 @@
         <v>82</v>
       </c>
       <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2039,8 +2051,11 @@
         <v>82</v>
       </c>
       <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2066,8 +2081,9 @@
       <c r="H5" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2093,8 +2109,11 @@
       <c r="H6" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2118,7 +2137,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2142,7 +2161,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2166,7 +2185,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -2190,7 +2209,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2216,8 +2235,11 @@
       <c r="H11" s="8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -2241,7 +2263,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2265,7 +2287,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2287,7 +2309,7 @@
       </c>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2313,8 +2335,11 @@
       <c r="H15" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -2338,7 +2363,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2364,8 +2389,11 @@
       <c r="H17" s="8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2388,8 +2416,11 @@
       <c r="H18" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2413,8 +2444,11 @@
       <c r="H19" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2441,7 +2475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2465,7 +2499,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2488,8 +2522,11 @@
       <c r="H22" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2513,8 +2550,11 @@
         <v>82</v>
       </c>
       <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2538,7 +2578,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2562,7 +2602,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2586,8 +2626,11 @@
         <v>82</v>
       </c>
       <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2610,6 +2653,9 @@
       <c r="G27" s="7"/>
       <c r="H27" s="8" t="s">
         <v>119</v>
+      </c>
+      <c r="I27" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2622,7 +2668,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>